<commit_message>
Fixed the lookahead heuristic
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -43,15 +43,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="32">
   <si>
     <t xml:space="preserve">Trivial Case </t>
   </si>
   <si>
     <t>ASt</t>
-  </si>
-  <si>
-    <t>cartesian)</t>
   </si>
   <si>
     <t xml:space="preserve">One Triangle </t>
@@ -114,9 +111,6 @@
     <t xml:space="preserve">Deja Vu </t>
   </si>
   <si>
-    <t>lookahead)</t>
-  </si>
-  <si>
     <t>GBF</t>
   </si>
   <si>
@@ -142,6 +136,9 @@
   </si>
   <si>
     <t>Iterations</t>
+  </si>
+  <si>
+    <t>lookahead</t>
   </si>
 </sst>
 </file>
@@ -499,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,70 +511,64 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>30</v>
-      </c>
-      <c r="D1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D2">
-        <v>11.313708498984701</v>
+        <v>12.3584854723722</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3">
-        <v>12.093368739633799</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4">
-        <v>12.6491106406735</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -585,27 +576,24 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5">
-        <v>11.313708498984701</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D6">
         <v>12.3584854723722</v>
@@ -616,627 +604,603 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7">
-        <v>30.488451223761</v>
-      </c>
-      <c r="E7">
-        <v>393</v>
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8">
-        <v>29.949979386555899</v>
-      </c>
-      <c r="E8">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9">
-        <v>32.387650199806799</v>
-      </c>
-      <c r="E9">
-        <v>36</v>
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" t="s">
-        <v>11</v>
+        <v>25</v>
+      </c>
+      <c r="D10">
+        <v>12.6491106406735</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D11">
-        <v>30.8600945056786</v>
+        <v>12.6491106406735</v>
       </c>
       <c r="E11">
-        <v>371</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D12">
-        <v>28.5643537898574</v>
+        <v>12.6491106406735</v>
       </c>
       <c r="E12">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D13">
-        <v>30.7861570503702</v>
+        <v>12.6491106406735</v>
       </c>
       <c r="E13">
-        <v>34</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D14">
-        <v>29.2069904766599</v>
+        <v>12.6491106406735</v>
       </c>
       <c r="E14">
-        <v>23</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D15">
-        <v>29.2409415537572</v>
+        <v>12.6491106406735</v>
       </c>
       <c r="E15">
-        <v>781</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D16">
-        <v>30.427603346441899</v>
+        <v>12.6491106406735</v>
       </c>
       <c r="E16">
-        <v>1183</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" t="s">
-        <v>11</v>
+        <v>31</v>
+      </c>
+      <c r="D17">
+        <v>12.6491106406735</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D18">
-        <v>31.521347176340399</v>
+        <v>30.488451223761</v>
       </c>
       <c r="E18">
-        <v>372</v>
+        <v>393</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20">
-        <v>26.294005679335001</v>
-      </c>
-      <c r="E20">
-        <v>12</v>
+        <v>25</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21">
-        <v>1051.7556884513599</v>
-      </c>
-      <c r="E21">
-        <v>37</v>
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B22" t="s">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D22">
-        <v>11.313708498984701</v>
+        <v>30.488451223761</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>393</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23">
-        <v>12.093368739633799</v>
-      </c>
-      <c r="E23">
-        <v>2</v>
+        <v>31</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24">
-        <v>12.6491106406735</v>
-      </c>
-      <c r="E24">
-        <v>4</v>
+        <v>31</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25">
-        <v>11.313708498984701</v>
-      </c>
-      <c r="E25">
-        <v>3</v>
+        <v>31</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D26">
-        <v>12.3584854723722</v>
+        <v>1051.7556884513599</v>
       </c>
       <c r="E26">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C27" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D27">
-        <v>30.488451223761</v>
+        <v>1201.7698730432801</v>
       </c>
       <c r="E27">
-        <v>393</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B28" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D28">
-        <v>29.949979386555899</v>
+        <v>1201.7698730432801</v>
       </c>
       <c r="E28">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D29">
-        <v>32.387650199806799</v>
+        <v>1320.0199923026801</v>
       </c>
       <c r="E29">
-        <v>36</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B30" t="s">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>23</v>
-      </c>
-      <c r="D30" t="s">
-        <v>11</v>
+        <v>31</v>
+      </c>
+      <c r="D30">
+        <v>1051.7556884513599</v>
+      </c>
+      <c r="E30">
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C31" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D31">
-        <v>30.8600945056786</v>
+        <v>1201.7698730432801</v>
       </c>
       <c r="E31">
-        <v>371</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B32" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D32">
-        <v>28.5643537898574</v>
+        <v>1201.7698730432801</v>
       </c>
       <c r="E32">
-        <v>19</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B33" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C33" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D33">
-        <v>30.7861570503702</v>
+        <v>1320.0199923026801</v>
       </c>
       <c r="E33">
-        <v>34</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B34" t="s">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D34">
-        <v>29.2069904766599</v>
+        <v>32.387650199806799</v>
       </c>
       <c r="E34">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C35" t="s">
-        <v>23</v>
-      </c>
-      <c r="D35">
-        <v>29.2409415537572</v>
-      </c>
-      <c r="E35">
-        <v>781</v>
+        <v>25</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B36" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C36" t="s">
-        <v>23</v>
-      </c>
-      <c r="D36">
-        <v>30.427603346441899</v>
-      </c>
-      <c r="E36">
-        <v>1183</v>
+        <v>25</v>
+      </c>
+      <c r="D36" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C37" t="s">
-        <v>23</v>
-      </c>
-      <c r="D37" t="s">
-        <v>11</v>
+        <v>25</v>
+      </c>
+      <c r="D37">
+        <v>42.365635077180997</v>
+      </c>
+      <c r="E37">
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B38" t="s">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D38">
-        <v>31.521347176340399</v>
+        <v>32.387650199806799</v>
       </c>
       <c r="E38">
-        <v>372</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C39" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C40" t="s">
-        <v>23</v>
-      </c>
-      <c r="D40">
-        <v>26.294005679335001</v>
-      </c>
-      <c r="E40">
-        <v>12</v>
+        <v>31</v>
+      </c>
+      <c r="D40" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C41" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D41">
-        <v>1051.7556884513599</v>
+        <v>39.705281007208796</v>
       </c>
       <c r="E41">
-        <v>37</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>2</v>
-      </c>
-      <c r="D42">
-        <v>11.313708498984701</v>
-      </c>
-      <c r="E42">
-        <v>1</v>
+        <v>25</v>
+      </c>
+      <c r="D42" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43">
+        <v>31.483123626630402</v>
+      </c>
+      <c r="E43">
         <v>3</v>
-      </c>
-      <c r="B43" t="s">
-        <v>24</v>
-      </c>
-      <c r="C43" t="s">
-        <v>2</v>
-      </c>
-      <c r="D43">
-        <v>12.093368739633799</v>
-      </c>
-      <c r="E43">
-        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C44" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D44">
-        <v>12.6491106406735</v>
+        <v>31.483123626630402</v>
       </c>
       <c r="E44">
         <v>2</v>
@@ -1244,16 +1208,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B45" t="s">
         <v>24</v>
       </c>
       <c r="C45" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D45">
-        <v>12.6491106406735</v>
+        <v>31.483123626630402</v>
       </c>
       <c r="E45">
         <v>2</v>
@@ -1261,47 +1225,50 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="D46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C47" t="s">
-        <v>2</v>
-      </c>
-      <c r="D47" t="s">
-        <v>11</v>
+        <v>31</v>
+      </c>
+      <c r="D47">
+        <v>31.483123626630402</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C48" t="s">
+        <v>31</v>
+      </c>
+      <c r="D48">
+        <v>31.483123626630402</v>
+      </c>
+      <c r="E48">
         <v>2</v>
-      </c>
-      <c r="D48">
-        <v>36.6118591069324</v>
-      </c>
-      <c r="E48">
-        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1312,38 +1279,41 @@
         <v>24</v>
       </c>
       <c r="C49" t="s">
+        <v>31</v>
+      </c>
+      <c r="D49">
+        <v>31.483123626630402</v>
+      </c>
+      <c r="E49">
         <v>2</v>
-      </c>
-      <c r="D49" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D50">
-        <v>31.483123626630402</v>
+        <v>30.8600945056786</v>
       </c>
       <c r="E50">
-        <v>3</v>
+        <v>371</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C51" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D51">
         <v>35.3903064624919</v>
@@ -1354,211 +1324,214 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C52" t="s">
-        <v>2</v>
-      </c>
-      <c r="D52">
-        <v>37.027756377319903</v>
-      </c>
-      <c r="E52">
-        <v>3</v>
+        <v>25</v>
+      </c>
+      <c r="D52" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B53" t="s">
         <v>24</v>
       </c>
       <c r="C53" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D53">
-        <v>37.498733967920998</v>
+        <v>33.6422423646966</v>
       </c>
       <c r="E53">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="D54">
-        <v>30.804112043605901</v>
+        <v>30.8600945056786</v>
       </c>
       <c r="E54">
-        <v>7</v>
+        <v>371</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C55" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="D55">
-        <v>32.320626387486001</v>
+        <v>35.3903064624919</v>
       </c>
       <c r="E55">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C56" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="D56" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B57" t="s">
         <v>24</v>
       </c>
       <c r="C57" t="s">
-        <v>2</v>
-      </c>
-      <c r="D57" t="s">
-        <v>11</v>
+        <v>31</v>
+      </c>
+      <c r="D57">
+        <v>33.6422423646966</v>
+      </c>
+      <c r="E57">
+        <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" t="s">
+        <v>25</v>
+      </c>
+      <c r="D58">
+        <v>28.5643537898574</v>
+      </c>
+      <c r="E58">
         <v>19</v>
-      </c>
-      <c r="B58" t="s">
-        <v>24</v>
-      </c>
-      <c r="C58" t="s">
-        <v>2</v>
-      </c>
-      <c r="D58">
-        <v>32.748605090273202</v>
-      </c>
-      <c r="E58">
-        <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B59" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C59" t="s">
-        <v>2</v>
-      </c>
-      <c r="D59" t="s">
-        <v>11</v>
+        <v>25</v>
+      </c>
+      <c r="D59">
+        <v>37.027756377319903</v>
+      </c>
+      <c r="E59">
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B60" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C60" t="s">
+        <v>25</v>
+      </c>
+      <c r="D60">
+        <v>37.027756377319903</v>
+      </c>
+      <c r="E60">
         <v>2</v>
-      </c>
-      <c r="D60">
-        <v>31.330797003598601</v>
-      </c>
-      <c r="E60">
-        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B61" t="s">
         <v>24</v>
       </c>
       <c r="C61" t="s">
+        <v>25</v>
+      </c>
+      <c r="D61">
+        <v>37.027756377319903</v>
+      </c>
+      <c r="E61">
         <v>2</v>
-      </c>
-      <c r="D61">
-        <v>1201.7698730432801</v>
-      </c>
-      <c r="E61">
-        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B62" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D62">
-        <v>11.313708498984701</v>
+        <v>28.5643537898574</v>
       </c>
       <c r="E62">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" t="s">
+        <v>22</v>
+      </c>
+      <c r="C63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D63">
+        <v>37.027756377319903</v>
+      </c>
+      <c r="E63">
         <v>3</v>
-      </c>
-      <c r="B63" t="s">
-        <v>24</v>
-      </c>
-      <c r="C63" t="s">
-        <v>23</v>
-      </c>
-      <c r="D63">
-        <v>12.093368739633799</v>
-      </c>
-      <c r="E63">
-        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B64" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C64" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D64">
-        <v>12.6491106406735</v>
+        <v>37.027756377319903</v>
       </c>
       <c r="E64">
         <v>2</v>
@@ -1566,16 +1539,16 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B65" t="s">
         <v>24</v>
       </c>
       <c r="C65" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D65">
-        <v>12.6491106406735</v>
+        <v>37.027756377319903</v>
       </c>
       <c r="E65">
         <v>2</v>
@@ -1583,95 +1556,104 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B66" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>23</v>
-      </c>
-      <c r="D66" t="s">
-        <v>11</v>
+        <v>25</v>
+      </c>
+      <c r="D66">
+        <v>30.7861570503702</v>
+      </c>
+      <c r="E66">
+        <v>34</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B67" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C67" t="s">
-        <v>23</v>
-      </c>
-      <c r="D67" t="s">
-        <v>11</v>
+        <v>25</v>
+      </c>
+      <c r="D67">
+        <v>37.498733967920998</v>
+      </c>
+      <c r="E67">
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B68" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C68" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D68">
-        <v>29.949979386555899</v>
+        <v>34.292985660078799</v>
       </c>
       <c r="E68">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B69" t="s">
         <v>24</v>
       </c>
       <c r="C69" t="s">
-        <v>23</v>
-      </c>
-      <c r="D69" t="s">
-        <v>11</v>
+        <v>25</v>
+      </c>
+      <c r="D69">
+        <v>37.498733967920998</v>
+      </c>
+      <c r="E69">
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B70" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D70">
-        <v>31.483123626630402</v>
+        <v>30.7861570503702</v>
       </c>
       <c r="E70">
-        <v>3</v>
+        <v>34</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B71" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C71" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D71">
-        <v>35.3903064624919</v>
+        <v>34.292985660078799</v>
       </c>
       <c r="E71">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -1679,30 +1661,30 @@
         <v>13</v>
       </c>
       <c r="B72" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C72" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D72">
-        <v>37.027756377319903</v>
+        <v>37.498733967920998</v>
       </c>
       <c r="E72">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B73" t="s">
         <v>24</v>
       </c>
       <c r="C73" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D73">
-        <v>34.292985660078799</v>
+        <v>37.498733967920998</v>
       </c>
       <c r="E73">
         <v>4</v>
@@ -1710,163 +1692,166 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B74" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C74" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D74">
-        <v>30.804112043605901</v>
+        <v>29.2069904766599</v>
       </c>
       <c r="E74">
-        <v>7</v>
+        <v>23</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B75" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C75" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D75">
-        <v>32.320626387486001</v>
+        <v>30.804112043605901</v>
       </c>
       <c r="E75">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B76" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C76" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D76" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B77" t="s">
         <v>24</v>
       </c>
       <c r="C77" t="s">
-        <v>23</v>
-      </c>
-      <c r="D77" t="s">
-        <v>11</v>
+        <v>25</v>
+      </c>
+      <c r="D77">
+        <v>29.9822657255168</v>
+      </c>
+      <c r="E77">
+        <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B78" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C78" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D78">
-        <v>32.748605090273202</v>
+        <v>29.2069904766599</v>
       </c>
       <c r="E78">
-        <v>7</v>
+        <v>23</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B79" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C79" t="s">
-        <v>23</v>
-      </c>
-      <c r="D79" t="s">
-        <v>11</v>
+        <v>31</v>
+      </c>
+      <c r="D79">
+        <v>30.804112043605901</v>
+      </c>
+      <c r="E79">
+        <v>7</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B80" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C80" t="s">
-        <v>23</v>
-      </c>
-      <c r="D80">
-        <v>31.330797003598601</v>
-      </c>
-      <c r="E80">
-        <v>4</v>
+        <v>31</v>
+      </c>
+      <c r="D80" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B81" t="s">
         <v>24</v>
       </c>
       <c r="C81" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D81">
-        <v>1201.7698730432801</v>
+        <v>29.9822657255168</v>
       </c>
       <c r="E81">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B82" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C82" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D82">
         <v>11.313708498984701</v>
       </c>
       <c r="E82">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B83" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C83" t="s">
+        <v>25</v>
+      </c>
+      <c r="D83">
+        <v>12.6491106406735</v>
+      </c>
+      <c r="E83">
         <v>2</v>
-      </c>
-      <c r="D83">
-        <v>12.093368739633799</v>
-      </c>
-      <c r="E83">
-        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -1874,10 +1859,10 @@
         <v>4</v>
       </c>
       <c r="B84" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C84" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D84">
         <v>12.6491106406735</v>
@@ -1888,13 +1873,13 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B85" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C85" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D85">
         <v>12.6491106406735</v>
@@ -1905,126 +1890,138 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B86" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C86" t="s">
-        <v>2</v>
-      </c>
-      <c r="D86" t="s">
-        <v>11</v>
+        <v>31</v>
+      </c>
+      <c r="D86">
+        <v>11.313708498984701</v>
+      </c>
+      <c r="E86">
+        <v>3</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B87" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C87" t="s">
+        <v>31</v>
+      </c>
+      <c r="D87">
+        <v>12.6491106406735</v>
+      </c>
+      <c r="E87">
         <v>2</v>
-      </c>
-      <c r="D87" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B88" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C88" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="D88">
-        <v>36.6118591069324</v>
+        <v>12.6491106406735</v>
       </c>
       <c r="E88">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B89" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C89" t="s">
-        <v>2</v>
-      </c>
-      <c r="D89" t="s">
-        <v>11</v>
+        <v>31</v>
+      </c>
+      <c r="D89">
+        <v>12.6491106406735</v>
+      </c>
+      <c r="E89">
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B90" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C90" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D90">
-        <v>31.483123626630402</v>
+        <v>29.2409415537572</v>
       </c>
       <c r="E90">
-        <v>2</v>
+        <v>781</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B91" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C91" t="s">
-        <v>2</v>
-      </c>
-      <c r="D91" t="s">
-        <v>11</v>
+        <v>25</v>
+      </c>
+      <c r="D91">
+        <v>32.320626387486001</v>
+      </c>
+      <c r="E91">
+        <v>6</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B92" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C92" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D92">
-        <v>37.027756377319903</v>
+        <v>32.320626387486001</v>
       </c>
       <c r="E92">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B93" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C93" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D93">
-        <v>34.292985660078799</v>
+        <v>35.038404810405297</v>
       </c>
       <c r="E93">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2032,360 +2029,348 @@
         <v>15</v>
       </c>
       <c r="B94" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C94" t="s">
-        <v>2</v>
-      </c>
-      <c r="D94" t="s">
-        <v>11</v>
+        <v>31</v>
+      </c>
+      <c r="D94">
+        <v>29.2409415537572</v>
+      </c>
+      <c r="E94">
+        <v>781</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B95" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C95" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="D95">
         <v>32.320626387486001</v>
       </c>
       <c r="E95">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B96" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C96" t="s">
-        <v>2</v>
-      </c>
-      <c r="D96" t="s">
-        <v>11</v>
+        <v>31</v>
+      </c>
+      <c r="D96">
+        <v>32.320626387486001</v>
+      </c>
+      <c r="E96">
+        <v>5</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B97" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C97" t="s">
-        <v>2</v>
-      </c>
-      <c r="D97" t="s">
-        <v>11</v>
+        <v>31</v>
+      </c>
+      <c r="D97">
+        <v>35.038404810405297</v>
+      </c>
+      <c r="E97">
+        <v>4</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B98" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C98" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D98">
-        <v>32.748605090273202</v>
+        <v>30.427603346441899</v>
       </c>
       <c r="E98">
-        <v>6</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B99" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C99" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D99" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B100" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C100" t="s">
-        <v>2</v>
-      </c>
-      <c r="D100">
-        <v>31.330797003598601</v>
-      </c>
-      <c r="E100">
-        <v>3</v>
+        <v>25</v>
+      </c>
+      <c r="D100" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B101" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C101" t="s">
-        <v>2</v>
-      </c>
-      <c r="D101">
-        <v>1201.7698730432801</v>
-      </c>
-      <c r="E101">
-        <v>4</v>
+        <v>25</v>
+      </c>
+      <c r="D101" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B102" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C102" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D102">
-        <v>11.313708498984701</v>
+        <v>30.427603346441899</v>
       </c>
       <c r="E102">
-        <v>0</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B103" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C103" t="s">
-        <v>23</v>
-      </c>
-      <c r="D103">
-        <v>12.093368739633799</v>
-      </c>
-      <c r="E103">
-        <v>1</v>
+        <v>31</v>
+      </c>
+      <c r="D103" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B104" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C104" t="s">
-        <v>23</v>
-      </c>
-      <c r="D104">
-        <v>12.6491106406735</v>
-      </c>
-      <c r="E104">
-        <v>1</v>
+        <v>31</v>
+      </c>
+      <c r="D104" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B105" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C105" t="s">
-        <v>23</v>
-      </c>
-      <c r="D105">
-        <v>12.6491106406735</v>
-      </c>
-      <c r="E105">
-        <v>1</v>
+        <v>31</v>
+      </c>
+      <c r="D105" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B106" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C106" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D106" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B107" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C107" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D107" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B108" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C108" t="s">
-        <v>23</v>
-      </c>
-      <c r="D108">
-        <v>29.949979386555899</v>
-      </c>
-      <c r="E108">
-        <v>3</v>
+        <v>25</v>
+      </c>
+      <c r="D108" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B109" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C109" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D109" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B110" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C110" t="s">
-        <v>23</v>
-      </c>
-      <c r="D110">
-        <v>31.483123626630402</v>
-      </c>
-      <c r="E110">
-        <v>2</v>
+        <v>31</v>
+      </c>
+      <c r="D110" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B111" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C111" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D111" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B112" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C112" t="s">
-        <v>23</v>
-      </c>
-      <c r="D112">
-        <v>37.027756377319903</v>
-      </c>
-      <c r="E112">
-        <v>2</v>
+        <v>31</v>
+      </c>
+      <c r="D112" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B113" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C113" t="s">
-        <v>23</v>
-      </c>
-      <c r="D113">
-        <v>37.498733967920998</v>
-      </c>
-      <c r="E113">
-        <v>4</v>
+        <v>31</v>
+      </c>
+      <c r="D113" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B114" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C114" t="s">
-        <v>23</v>
-      </c>
-      <c r="D114" t="s">
-        <v>11</v>
+        <v>25</v>
+      </c>
+      <c r="D114">
+        <v>31.521347176340399</v>
+      </c>
+      <c r="E114">
+        <v>372</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B115" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C115" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D115">
-        <v>32.320626387486001</v>
+        <v>32.748605090273202</v>
       </c>
       <c r="E115">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B116" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C116" t="s">
-        <v>23</v>
-      </c>
-      <c r="D116" t="s">
-        <v>11</v>
+        <v>25</v>
+      </c>
+      <c r="D116">
+        <v>32.748605090273202</v>
+      </c>
+      <c r="E116">
+        <v>6</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -2393,307 +2378,295 @@
         <v>18</v>
       </c>
       <c r="B117" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C117" t="s">
-        <v>23</v>
-      </c>
-      <c r="D117" t="s">
-        <v>11</v>
+        <v>25</v>
+      </c>
+      <c r="D117">
+        <v>31.521347176340399</v>
+      </c>
+      <c r="E117">
+        <v>5</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B118" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C118" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D118">
-        <v>32.748605090273202</v>
+        <v>31.521347176340399</v>
       </c>
       <c r="E118">
-        <v>6</v>
+        <v>372</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B119" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C119" t="s">
-        <v>23</v>
-      </c>
-      <c r="D119" t="s">
-        <v>11</v>
+        <v>31</v>
+      </c>
+      <c r="D119">
+        <v>32.748605090273202</v>
+      </c>
+      <c r="E119">
+        <v>7</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B120" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C120" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D120">
-        <v>31.330797003598601</v>
+        <v>32.748605090273202</v>
       </c>
       <c r="E120">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B121" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C121" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D121">
-        <v>1201.7698730432801</v>
+        <v>31.521347176340399</v>
       </c>
       <c r="E121">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B122" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="C122" t="s">
-        <v>2</v>
-      </c>
-      <c r="D122">
-        <v>11.313708498984701</v>
-      </c>
-      <c r="E122">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="D122" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B123" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C123" t="s">
-        <v>2</v>
-      </c>
-      <c r="D123">
-        <v>12.093368739633799</v>
-      </c>
-      <c r="E123">
-        <v>1</v>
+        <v>25</v>
+      </c>
+      <c r="D123" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B124" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C124" t="s">
-        <v>2</v>
-      </c>
-      <c r="D124">
-        <v>12.6491106406735</v>
-      </c>
-      <c r="E124">
-        <v>1</v>
+        <v>25</v>
+      </c>
+      <c r="D124" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B125" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C125" t="s">
-        <v>2</v>
-      </c>
-      <c r="D125">
-        <v>12.6491106406735</v>
-      </c>
-      <c r="E125">
-        <v>1</v>
+        <v>25</v>
+      </c>
+      <c r="D125" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B126" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="C126" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="D126" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B127" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C127" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="D127" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B128" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C128" t="s">
-        <v>2</v>
-      </c>
-      <c r="D128">
-        <v>29.949979386555899</v>
-      </c>
-      <c r="E128">
-        <v>3</v>
+        <v>31</v>
+      </c>
+      <c r="D128" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B129" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C129" t="s">
-        <v>2</v>
-      </c>
-      <c r="D129">
-        <v>42.365635077180997</v>
-      </c>
-      <c r="E129">
-        <v>5</v>
+        <v>31</v>
+      </c>
+      <c r="D129" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B130" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="C130" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D130">
-        <v>31.483123626630402</v>
+        <v>26.294005679335001</v>
       </c>
       <c r="E130">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B131" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C131" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D131">
-        <v>33.6422423646966</v>
+        <v>31.330797003598601</v>
       </c>
       <c r="E131">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B132" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C132" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D132">
-        <v>37.027756377319903</v>
+        <v>31.330797003598601</v>
       </c>
       <c r="E132">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B133" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C133" t="s">
+        <v>25</v>
+      </c>
+      <c r="D133">
+        <v>29.699304983972301</v>
+      </c>
+      <c r="E133">
         <v>2</v>
-      </c>
-      <c r="D133">
-        <v>37.498733967920998</v>
-      </c>
-      <c r="E133">
-        <v>4</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B134" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="C134" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="D134">
-        <v>29.9822657255168</v>
+        <v>26.294005679335001</v>
       </c>
       <c r="E134">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B135" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C135" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="D135">
-        <v>35.038404810405297</v>
+        <v>31.330797003598601</v>
       </c>
       <c r="E135">
         <v>4</v>
@@ -2701,143 +2674,152 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B136" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C136" t="s">
-        <v>2</v>
-      </c>
-      <c r="D136" t="s">
-        <v>11</v>
+        <v>31</v>
+      </c>
+      <c r="D136">
+        <v>31.330797003598601</v>
+      </c>
+      <c r="E136">
+        <v>3</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B137" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C137" t="s">
+        <v>31</v>
+      </c>
+      <c r="D137">
+        <v>29.699304983972301</v>
+      </c>
+      <c r="E137">
         <v>2</v>
-      </c>
-      <c r="D137" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="B138" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="C138" t="s">
+        <v>25</v>
+      </c>
+      <c r="D138">
+        <v>12.093368739633799</v>
+      </c>
+      <c r="E138">
         <v>2</v>
-      </c>
-      <c r="D138">
-        <v>31.521347176340399</v>
-      </c>
-      <c r="E138">
-        <v>5</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B139" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C139" t="s">
+        <v>25</v>
+      </c>
+      <c r="D139">
+        <v>12.093368739633799</v>
+      </c>
+      <c r="E139">
         <v>2</v>
-      </c>
-      <c r="D139" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="B140" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C140" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D140">
-        <v>29.699304983972301</v>
+        <v>12.093368739633799</v>
       </c>
       <c r="E140">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B141" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C141" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D141">
-        <v>1320.0199923026801</v>
+        <v>12.093368739633799</v>
       </c>
       <c r="E141">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B142" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="C142" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D142">
-        <v>11.313708498984701</v>
+        <v>12.093368739633799</v>
       </c>
       <c r="E142">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B143" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C143" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D143">
         <v>12.093368739633799</v>
       </c>
       <c r="E143">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B144" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C144" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D144">
-        <v>12.6491106406735</v>
+        <v>12.093368739633799</v>
       </c>
       <c r="E144">
         <v>1</v>
@@ -2845,16 +2827,16 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B145" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C145" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D145">
-        <v>12.6491106406735</v>
+        <v>12.093368739633799</v>
       </c>
       <c r="E145">
         <v>1</v>
@@ -2862,16 +2844,19 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B146" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="C146" t="s">
-        <v>23</v>
-      </c>
-      <c r="D146" t="s">
-        <v>11</v>
+        <v>25</v>
+      </c>
+      <c r="D146">
+        <v>29.949979386555899</v>
+      </c>
+      <c r="E146">
+        <v>8</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -2879,245 +2864,260 @@
         <v>7</v>
       </c>
       <c r="B147" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C147" t="s">
-        <v>23</v>
-      </c>
-      <c r="D147" t="s">
-        <v>11</v>
+        <v>25</v>
+      </c>
+      <c r="D147">
+        <v>36.6118591069324</v>
+      </c>
+      <c r="E147">
+        <v>5</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B148" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C148" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D148">
-        <v>29.949979386555899</v>
+        <v>36.6118591069324</v>
       </c>
       <c r="E148">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B149" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C149" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D149">
-        <v>39.705281007208796</v>
+        <v>29.949979386555899</v>
       </c>
       <c r="E149">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B150" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="C150" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D150">
-        <v>31.483123626630402</v>
+        <v>29.949979386555899</v>
       </c>
       <c r="E150">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B151" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C151" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D151">
-        <v>33.6422423646966</v>
+        <v>29.949979386555899</v>
       </c>
       <c r="E151">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B152" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C152" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D152">
-        <v>37.027756377319903</v>
+        <v>29.949979386555899</v>
       </c>
       <c r="E152">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B153" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C153" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D153">
-        <v>37.498733967920998</v>
+        <v>29.949979386555899</v>
       </c>
       <c r="E153">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B154" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="C154" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D154">
-        <v>29.9822657255168</v>
+        <v>11.313708498984701</v>
       </c>
       <c r="E154">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B155" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C155" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D155">
-        <v>35.038404810405297</v>
+        <v>11.313708498984701</v>
       </c>
       <c r="E155">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B156" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C156" t="s">
-        <v>23</v>
-      </c>
-      <c r="D156" t="s">
-        <v>11</v>
+        <v>25</v>
+      </c>
+      <c r="D156">
+        <v>11.313708498984701</v>
+      </c>
+      <c r="E156">
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B157" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C157" t="s">
-        <v>23</v>
-      </c>
-      <c r="D157" t="s">
-        <v>11</v>
+        <v>25</v>
+      </c>
+      <c r="D157">
+        <v>11.313708498984701</v>
+      </c>
+      <c r="E157">
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B158" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="C158" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D158">
-        <v>31.521347176340399</v>
+        <v>11.313708498984701</v>
       </c>
       <c r="E158">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B159" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C159" t="s">
-        <v>23</v>
-      </c>
-      <c r="D159" t="s">
-        <v>11</v>
+        <v>31</v>
+      </c>
+      <c r="D159">
+        <v>11.313708498984701</v>
+      </c>
+      <c r="E159">
+        <v>1</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B160" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C160" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D160">
-        <v>29.699304983972301</v>
+        <v>11.313708498984701</v>
       </c>
       <c r="E160">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B161" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C161" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D161">
-        <v>1320.0199923026801</v>
+        <v>11.313708498984701</v>
       </c>
       <c r="E161">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:E161">
+    <sortCondition ref="A2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated data (excel worksheet) using recent fixes to hillclimbing and the lookahead heuristic
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -16,6 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="output" localSheetId="0">Sheet1!$A$2:$E$161</definedName>
+    <definedName name="output_1" localSheetId="0">Sheet1!$A$1:$E$160</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -39,11 +40,22 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="2" name="output1" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\Ananda\Documents\ai-final-project-path-navigation\output\output.txt" tab="0" comma="1" delimiter="(">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="27">
   <si>
     <t xml:space="preserve">Trivial Case </t>
   </si>
@@ -123,21 +135,6 @@
     <t>cartesian</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Algorithm</t>
-  </si>
-  <si>
-    <t>Heuristic</t>
-  </si>
-  <si>
-    <t>Length</t>
-  </si>
-  <si>
-    <t>Iterations</t>
-  </si>
-  <si>
     <t>lookahead</t>
   </si>
 </sst>
@@ -194,6 +191,10 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="output_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="output" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -494,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E161"/>
+  <dimension ref="A1:E160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,24 +507,24 @@
     <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" t="s">
-        <v>30</v>
+        <v>25</v>
+      </c>
+      <c r="D1">
+        <v>12.3584854723722</v>
+      </c>
+      <c r="E1">
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -531,16 +532,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
       </c>
-      <c r="D2">
-        <v>12.3584854723722</v>
-      </c>
-      <c r="E2">
-        <v>53</v>
+      <c r="D2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -548,7 +546,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
@@ -562,7 +560,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
@@ -576,13 +574,16 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
+        <v>26</v>
+      </c>
+      <c r="D5">
+        <v>12.3584854723722</v>
+      </c>
+      <c r="E5">
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -590,16 +591,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6">
-        <v>12.3584854723722</v>
-      </c>
-      <c r="E6">
-        <v>53</v>
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -607,10 +605,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
@@ -621,10 +619,10 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -632,16 +630,19 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
+        <v>25</v>
+      </c>
+      <c r="D9">
+        <v>12.6491106406735</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -649,7 +650,7 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
         <v>25</v>
@@ -658,7 +659,7 @@
         <v>12.6491106406735</v>
       </c>
       <c r="E10">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -666,7 +667,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
         <v>25</v>
@@ -683,7 +684,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
         <v>25</v>
@@ -692,7 +693,7 @@
         <v>12.6491106406735</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -700,16 +701,16 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D13">
         <v>12.6491106406735</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -717,16 +718,16 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D14">
         <v>12.6491106406735</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -734,10 +735,10 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D15">
         <v>12.6491106406735</v>
@@ -751,33 +752,33 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D16">
         <v>12.6491106406735</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D17">
-        <v>12.6491106406735</v>
+        <v>30.488451223761</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>393</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -785,16 +786,13 @@
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C18" t="s">
         <v>25</v>
       </c>
-      <c r="D18">
-        <v>30.488451223761</v>
-      </c>
-      <c r="E18">
-        <v>393</v>
+      <c r="D18" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -802,7 +800,7 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
         <v>25</v>
@@ -816,7 +814,7 @@
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
@@ -830,13 +828,16 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" t="s">
-        <v>10</v>
+        <v>26</v>
+      </c>
+      <c r="D21">
+        <v>30.488451223761</v>
+      </c>
+      <c r="E21">
+        <v>393</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -844,16 +845,13 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22">
-        <v>30.488451223761</v>
-      </c>
-      <c r="E22">
-        <v>393</v>
+        <v>26</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -861,10 +859,10 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D23" t="s">
         <v>10</v>
@@ -875,10 +873,10 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D24" t="s">
         <v>10</v>
@@ -886,16 +884,19 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" t="s">
-        <v>10</v>
+        <v>25</v>
+      </c>
+      <c r="D25">
+        <v>1051.7556884513599</v>
+      </c>
+      <c r="E25">
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -903,16 +904,16 @@
         <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C26" t="s">
         <v>25</v>
       </c>
       <c r="D26">
-        <v>1051.7556884513599</v>
+        <v>1201.7698730432801</v>
       </c>
       <c r="E26">
-        <v>37</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -920,7 +921,7 @@
         <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C27" t="s">
         <v>25</v>
@@ -937,16 +938,16 @@
         <v>21</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C28" t="s">
         <v>25</v>
       </c>
       <c r="D28">
-        <v>1201.7698730432801</v>
+        <v>1320.0199923026801</v>
       </c>
       <c r="E28">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -954,16 +955,16 @@
         <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D29">
-        <v>1320.0199923026801</v>
+        <v>1051.7556884513599</v>
       </c>
       <c r="E29">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -971,16 +972,16 @@
         <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C30" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D30">
-        <v>1051.7556884513599</v>
+        <v>1201.7698730432801</v>
       </c>
       <c r="E30">
-        <v>37</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -988,10 +989,10 @@
         <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C31" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D31">
         <v>1201.7698730432801</v>
@@ -1005,33 +1006,33 @@
         <v>21</v>
       </c>
       <c r="B32" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C32" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D32">
-        <v>1201.7698730432801</v>
+        <v>1320.0199923026801</v>
       </c>
       <c r="E32">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D33">
-        <v>1320.0199923026801</v>
+        <v>32.387650199806799</v>
       </c>
       <c r="E33">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1039,16 +1040,13 @@
         <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C34" t="s">
         <v>25</v>
       </c>
-      <c r="D34">
-        <v>32.387650199806799</v>
-      </c>
-      <c r="E34">
-        <v>36</v>
+      <c r="D34" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1056,7 +1054,7 @@
         <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C35" t="s">
         <v>25</v>
@@ -1070,13 +1068,16 @@
         <v>8</v>
       </c>
       <c r="B36" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C36" t="s">
         <v>25</v>
       </c>
-      <c r="D36" t="s">
-        <v>10</v>
+      <c r="D36">
+        <v>42.365635077180997</v>
+      </c>
+      <c r="E36">
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1084,16 +1085,16 @@
         <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D37">
-        <v>42.365635077180997</v>
+        <v>32.387650199806799</v>
       </c>
       <c r="E37">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1101,16 +1102,13 @@
         <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D38">
-        <v>32.387650199806799</v>
-      </c>
-      <c r="E38">
-        <v>36</v>
+        <v>26</v>
+      </c>
+      <c r="D38" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1118,10 +1116,10 @@
         <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C39" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D39" t="s">
         <v>10</v>
@@ -1132,30 +1130,30 @@
         <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C40" t="s">
-        <v>31</v>
-      </c>
-      <c r="D40" t="s">
-        <v>10</v>
+        <v>26</v>
+      </c>
+      <c r="D40">
+        <v>39.705281007208796</v>
+      </c>
+      <c r="E40">
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>31</v>
-      </c>
-      <c r="D41">
-        <v>39.705281007208796</v>
-      </c>
-      <c r="E41">
-        <v>7</v>
+        <v>25</v>
+      </c>
+      <c r="D41" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1163,13 +1161,16 @@
         <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C42" t="s">
         <v>25</v>
       </c>
-      <c r="D42" t="s">
-        <v>10</v>
+      <c r="D42">
+        <v>31.483123626630402</v>
+      </c>
+      <c r="E42">
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1177,7 +1178,7 @@
         <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C43" t="s">
         <v>25</v>
@@ -1194,7 +1195,7 @@
         <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C44" t="s">
         <v>25</v>
@@ -1203,7 +1204,7 @@
         <v>31.483123626630402</v>
       </c>
       <c r="E44">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1211,16 +1212,13 @@
         <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>25</v>
-      </c>
-      <c r="D45">
-        <v>31.483123626630402</v>
-      </c>
-      <c r="E45">
-        <v>2</v>
+        <v>26</v>
+      </c>
+      <c r="D45" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1228,13 +1226,16 @@
         <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C46" t="s">
-        <v>31</v>
-      </c>
-      <c r="D46" t="s">
-        <v>10</v>
+        <v>26</v>
+      </c>
+      <c r="D46">
+        <v>31.483123626630402</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1242,10 +1243,10 @@
         <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C47" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D47">
         <v>31.483123626630402</v>
@@ -1259,33 +1260,33 @@
         <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C48" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D48">
         <v>31.483123626630402</v>
       </c>
       <c r="E48">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D49">
-        <v>31.483123626630402</v>
+        <v>30.8600945056786</v>
       </c>
       <c r="E49">
-        <v>2</v>
+        <v>371</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1293,16 +1294,16 @@
         <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C50" t="s">
         <v>25</v>
       </c>
       <c r="D50">
-        <v>30.8600945056786</v>
+        <v>35.3903064624919</v>
       </c>
       <c r="E50">
-        <v>371</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1310,16 +1311,13 @@
         <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C51" t="s">
         <v>25</v>
       </c>
-      <c r="D51">
-        <v>35.3903064624919</v>
-      </c>
-      <c r="E51">
-        <v>7</v>
+      <c r="D51" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1327,13 +1325,16 @@
         <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C52" t="s">
         <v>25</v>
       </c>
-      <c r="D52" t="s">
-        <v>10</v>
+      <c r="D52">
+        <v>33.6422423646966</v>
+      </c>
+      <c r="E52">
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1341,16 +1342,16 @@
         <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D53">
-        <v>33.6422423646966</v>
+        <v>30.8600945056786</v>
       </c>
       <c r="E53">
-        <v>6</v>
+        <v>371</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1358,16 +1359,16 @@
         <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C54" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D54">
-        <v>30.8600945056786</v>
+        <v>35.3903064624919</v>
       </c>
       <c r="E54">
-        <v>371</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1375,16 +1376,13 @@
         <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C55" t="s">
-        <v>31</v>
-      </c>
-      <c r="D55">
-        <v>35.3903064624919</v>
-      </c>
-      <c r="E55">
-        <v>7</v>
+        <v>26</v>
+      </c>
+      <c r="D55" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1392,30 +1390,33 @@
         <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C56" t="s">
-        <v>31</v>
-      </c>
-      <c r="D56" t="s">
-        <v>10</v>
+        <v>26</v>
+      </c>
+      <c r="D56">
+        <v>33.6422423646966</v>
+      </c>
+      <c r="E56">
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B57" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D57">
-        <v>33.6422423646966</v>
+        <v>28.5643537898574</v>
       </c>
       <c r="E57">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1423,16 +1424,16 @@
         <v>12</v>
       </c>
       <c r="B58" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C58" t="s">
         <v>25</v>
       </c>
       <c r="D58">
-        <v>28.5643537898574</v>
+        <v>37.027756377319903</v>
       </c>
       <c r="E58">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1440,7 +1441,7 @@
         <v>12</v>
       </c>
       <c r="B59" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C59" t="s">
         <v>25</v>
@@ -1457,7 +1458,7 @@
         <v>12</v>
       </c>
       <c r="B60" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C60" t="s">
         <v>25</v>
@@ -1466,7 +1467,7 @@
         <v>37.027756377319903</v>
       </c>
       <c r="E60">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -1474,16 +1475,16 @@
         <v>12</v>
       </c>
       <c r="B61" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D61">
-        <v>37.027756377319903</v>
+        <v>28.5643537898574</v>
       </c>
       <c r="E61">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1491,16 +1492,16 @@
         <v>12</v>
       </c>
       <c r="B62" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C62" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D62">
-        <v>28.5643537898574</v>
+        <v>37.027756377319903</v>
       </c>
       <c r="E62">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1508,10 +1509,10 @@
         <v>12</v>
       </c>
       <c r="B63" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C63" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D63">
         <v>37.027756377319903</v>
@@ -1525,33 +1526,33 @@
         <v>12</v>
       </c>
       <c r="B64" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C64" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D64">
         <v>37.027756377319903</v>
       </c>
       <c r="E64">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B65" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D65">
-        <v>37.027756377319903</v>
+        <v>30.7861570503702</v>
       </c>
       <c r="E65">
-        <v>2</v>
+        <v>34</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -1559,16 +1560,16 @@
         <v>13</v>
       </c>
       <c r="B66" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C66" t="s">
         <v>25</v>
       </c>
       <c r="D66">
-        <v>30.7861570503702</v>
+        <v>37.498733967920998</v>
       </c>
       <c r="E66">
-        <v>34</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -1576,16 +1577,16 @@
         <v>13</v>
       </c>
       <c r="B67" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C67" t="s">
         <v>25</v>
       </c>
       <c r="D67">
-        <v>37.498733967920998</v>
+        <v>34.292985660078799</v>
       </c>
       <c r="E67">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -1593,16 +1594,16 @@
         <v>13</v>
       </c>
       <c r="B68" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C68" t="s">
         <v>25</v>
       </c>
       <c r="D68">
-        <v>34.292985660078799</v>
+        <v>37.498733967920998</v>
       </c>
       <c r="E68">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -1610,16 +1611,16 @@
         <v>13</v>
       </c>
       <c r="B69" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D69">
-        <v>37.498733967920998</v>
+        <v>30.7861570503702</v>
       </c>
       <c r="E69">
-        <v>4</v>
+        <v>34</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -1627,16 +1628,16 @@
         <v>13</v>
       </c>
       <c r="B70" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C70" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D70">
-        <v>30.7861570503702</v>
+        <v>34.292985660078799</v>
       </c>
       <c r="E70">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -1644,16 +1645,16 @@
         <v>13</v>
       </c>
       <c r="B71" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C71" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D71">
-        <v>34.292985660078799</v>
+        <v>37.498733967920998</v>
       </c>
       <c r="E71">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -1661,33 +1662,33 @@
         <v>13</v>
       </c>
       <c r="B72" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C72" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D72">
         <v>37.498733967920998</v>
       </c>
       <c r="E72">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B73" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C73" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D73">
-        <v>37.498733967920998</v>
+        <v>29.2069904766599</v>
       </c>
       <c r="E73">
-        <v>4</v>
+        <v>23</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -1695,16 +1696,16 @@
         <v>14</v>
       </c>
       <c r="B74" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C74" t="s">
         <v>25</v>
       </c>
       <c r="D74">
-        <v>29.2069904766599</v>
+        <v>30.804112043605901</v>
       </c>
       <c r="E74">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -1712,16 +1713,13 @@
         <v>14</v>
       </c>
       <c r="B75" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C75" t="s">
         <v>25</v>
       </c>
-      <c r="D75">
-        <v>30.804112043605901</v>
-      </c>
-      <c r="E75">
-        <v>7</v>
+      <c r="D75" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -1729,13 +1727,16 @@
         <v>14</v>
       </c>
       <c r="B76" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C76" t="s">
         <v>25</v>
       </c>
-      <c r="D76" t="s">
-        <v>10</v>
+      <c r="D76">
+        <v>29.9822657255168</v>
+      </c>
+      <c r="E76">
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -1743,16 +1744,16 @@
         <v>14</v>
       </c>
       <c r="B77" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C77" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D77">
-        <v>29.9822657255168</v>
+        <v>29.2069904766599</v>
       </c>
       <c r="E77">
-        <v>4</v>
+        <v>23</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -1760,16 +1761,16 @@
         <v>14</v>
       </c>
       <c r="B78" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C78" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D78">
-        <v>29.2069904766599</v>
+        <v>30.804112043605901</v>
       </c>
       <c r="E78">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -1777,16 +1778,13 @@
         <v>14</v>
       </c>
       <c r="B79" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C79" t="s">
-        <v>31</v>
-      </c>
-      <c r="D79">
-        <v>30.804112043605901</v>
-      </c>
-      <c r="E79">
-        <v>7</v>
+        <v>26</v>
+      </c>
+      <c r="D79" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -1794,30 +1792,33 @@
         <v>14</v>
       </c>
       <c r="B80" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C80" t="s">
-        <v>31</v>
-      </c>
-      <c r="D80" t="s">
-        <v>10</v>
+        <v>26</v>
+      </c>
+      <c r="D80">
+        <v>32.252697129720197</v>
+      </c>
+      <c r="E80">
+        <v>6</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B81" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C81" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D81">
-        <v>29.9822657255168</v>
+        <v>11.313708498984701</v>
       </c>
       <c r="E81">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -1825,16 +1826,16 @@
         <v>4</v>
       </c>
       <c r="B82" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C82" t="s">
         <v>25</v>
       </c>
       <c r="D82">
-        <v>11.313708498984701</v>
+        <v>12.6491106406735</v>
       </c>
       <c r="E82">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -1842,7 +1843,7 @@
         <v>4</v>
       </c>
       <c r="B83" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C83" t="s">
         <v>25</v>
@@ -1859,7 +1860,7 @@
         <v>4</v>
       </c>
       <c r="B84" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C84" t="s">
         <v>25</v>
@@ -1868,7 +1869,7 @@
         <v>12.6491106406735</v>
       </c>
       <c r="E84">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -1876,16 +1877,16 @@
         <v>4</v>
       </c>
       <c r="B85" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C85" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D85">
-        <v>12.6491106406735</v>
+        <v>11.313708498984701</v>
       </c>
       <c r="E85">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -1893,16 +1894,16 @@
         <v>4</v>
       </c>
       <c r="B86" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C86" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D86">
-        <v>11.313708498984701</v>
+        <v>12.6491106406735</v>
       </c>
       <c r="E86">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -1910,10 +1911,10 @@
         <v>4</v>
       </c>
       <c r="B87" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C87" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D87">
         <v>12.6491106406735</v>
@@ -1927,33 +1928,33 @@
         <v>4</v>
       </c>
       <c r="B88" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C88" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D88">
         <v>12.6491106406735</v>
       </c>
       <c r="E88">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B89" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C89" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D89">
-        <v>12.6491106406735</v>
+        <v>29.2409415537572</v>
       </c>
       <c r="E89">
-        <v>1</v>
+        <v>781</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -1961,16 +1962,16 @@
         <v>15</v>
       </c>
       <c r="B90" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C90" t="s">
         <v>25</v>
       </c>
       <c r="D90">
-        <v>29.2409415537572</v>
+        <v>32.320626387486001</v>
       </c>
       <c r="E90">
-        <v>781</v>
+        <v>6</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -1978,7 +1979,7 @@
         <v>15</v>
       </c>
       <c r="B91" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C91" t="s">
         <v>25</v>
@@ -1995,13 +1996,13 @@
         <v>15</v>
       </c>
       <c r="B92" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C92" t="s">
         <v>25</v>
       </c>
       <c r="D92">
-        <v>32.320626387486001</v>
+        <v>35.038404810405297</v>
       </c>
       <c r="E92">
         <v>5</v>
@@ -2012,16 +2013,16 @@
         <v>15</v>
       </c>
       <c r="B93" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C93" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D93">
-        <v>35.038404810405297</v>
+        <v>29.2409415537572</v>
       </c>
       <c r="E93">
-        <v>4</v>
+        <v>781</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2029,16 +2030,16 @@
         <v>15</v>
       </c>
       <c r="B94" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C94" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D94">
-        <v>29.2409415537572</v>
+        <v>32.320626387486001</v>
       </c>
       <c r="E94">
-        <v>781</v>
+        <v>6</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -2046,10 +2047,10 @@
         <v>15</v>
       </c>
       <c r="B95" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C95" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D95">
         <v>32.320626387486001</v>
@@ -2063,13 +2064,13 @@
         <v>15</v>
       </c>
       <c r="B96" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C96" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D96">
-        <v>32.320626387486001</v>
+        <v>35.038404810405297</v>
       </c>
       <c r="E96">
         <v>5</v>
@@ -2077,19 +2078,19 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B97" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C97" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D97">
-        <v>35.038404810405297</v>
+        <v>30.427603346441899</v>
       </c>
       <c r="E97">
-        <v>4</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2097,16 +2098,13 @@
         <v>16</v>
       </c>
       <c r="B98" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C98" t="s">
         <v>25</v>
       </c>
-      <c r="D98">
-        <v>30.427603346441899</v>
-      </c>
-      <c r="E98">
-        <v>1183</v>
+      <c r="D98" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2114,7 +2112,7 @@
         <v>16</v>
       </c>
       <c r="B99" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C99" t="s">
         <v>25</v>
@@ -2128,7 +2126,7 @@
         <v>16</v>
       </c>
       <c r="B100" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C100" t="s">
         <v>25</v>
@@ -2142,13 +2140,16 @@
         <v>16</v>
       </c>
       <c r="B101" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C101" t="s">
-        <v>25</v>
-      </c>
-      <c r="D101" t="s">
-        <v>10</v>
+        <v>26</v>
+      </c>
+      <c r="D101">
+        <v>30.427603346441899</v>
+      </c>
+      <c r="E101">
+        <v>1183</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2156,16 +2157,13 @@
         <v>16</v>
       </c>
       <c r="B102" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C102" t="s">
-        <v>31</v>
-      </c>
-      <c r="D102">
-        <v>30.427603346441899</v>
-      </c>
-      <c r="E102">
-        <v>1183</v>
+        <v>26</v>
+      </c>
+      <c r="D102" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2173,10 +2171,10 @@
         <v>16</v>
       </c>
       <c r="B103" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C103" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D103" t="s">
         <v>10</v>
@@ -2187,10 +2185,10 @@
         <v>16</v>
       </c>
       <c r="B104" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C104" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D104" t="s">
         <v>10</v>
@@ -2198,13 +2196,13 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B105" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C105" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D105" t="s">
         <v>10</v>
@@ -2215,7 +2213,7 @@
         <v>17</v>
       </c>
       <c r="B106" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C106" t="s">
         <v>25</v>
@@ -2229,7 +2227,7 @@
         <v>17</v>
       </c>
       <c r="B107" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C107" t="s">
         <v>25</v>
@@ -2243,7 +2241,7 @@
         <v>17</v>
       </c>
       <c r="B108" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C108" t="s">
         <v>25</v>
@@ -2257,10 +2255,10 @@
         <v>17</v>
       </c>
       <c r="B109" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C109" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D109" t="s">
         <v>10</v>
@@ -2271,10 +2269,10 @@
         <v>17</v>
       </c>
       <c r="B110" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C110" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D110" t="s">
         <v>10</v>
@@ -2285,10 +2283,10 @@
         <v>17</v>
       </c>
       <c r="B111" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C111" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D111" t="s">
         <v>10</v>
@@ -2299,10 +2297,10 @@
         <v>17</v>
       </c>
       <c r="B112" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C112" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D112" t="s">
         <v>10</v>
@@ -2310,16 +2308,19 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B113" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C113" t="s">
-        <v>31</v>
-      </c>
-      <c r="D113" t="s">
-        <v>10</v>
+        <v>25</v>
+      </c>
+      <c r="D113">
+        <v>31.521347176340399</v>
+      </c>
+      <c r="E113">
+        <v>372</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -2327,16 +2328,16 @@
         <v>18</v>
       </c>
       <c r="B114" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C114" t="s">
         <v>25</v>
       </c>
       <c r="D114">
-        <v>31.521347176340399</v>
+        <v>32.748605090273202</v>
       </c>
       <c r="E114">
-        <v>372</v>
+        <v>7</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -2344,7 +2345,7 @@
         <v>18</v>
       </c>
       <c r="B115" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C115" t="s">
         <v>25</v>
@@ -2361,13 +2362,13 @@
         <v>18</v>
       </c>
       <c r="B116" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C116" t="s">
         <v>25</v>
       </c>
       <c r="D116">
-        <v>32.748605090273202</v>
+        <v>31.521347176340399</v>
       </c>
       <c r="E116">
         <v>6</v>
@@ -2378,16 +2379,16 @@
         <v>18</v>
       </c>
       <c r="B117" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C117" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D117">
         <v>31.521347176340399</v>
       </c>
       <c r="E117">
-        <v>5</v>
+        <v>372</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -2395,16 +2396,16 @@
         <v>18</v>
       </c>
       <c r="B118" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C118" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D118">
-        <v>31.521347176340399</v>
+        <v>32.748605090273202</v>
       </c>
       <c r="E118">
-        <v>372</v>
+        <v>7</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -2412,10 +2413,10 @@
         <v>18</v>
       </c>
       <c r="B119" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C119" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D119">
         <v>32.748605090273202</v>
@@ -2429,13 +2430,13 @@
         <v>18</v>
       </c>
       <c r="B120" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C120" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D120">
-        <v>32.748605090273202</v>
+        <v>31.521347176340399</v>
       </c>
       <c r="E120">
         <v>6</v>
@@ -2443,19 +2444,16 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B121" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C121" t="s">
-        <v>31</v>
-      </c>
-      <c r="D121">
-        <v>31.521347176340399</v>
-      </c>
-      <c r="E121">
-        <v>5</v>
+        <v>25</v>
+      </c>
+      <c r="D121" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -2463,7 +2461,7 @@
         <v>19</v>
       </c>
       <c r="B122" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C122" t="s">
         <v>25</v>
@@ -2477,7 +2475,7 @@
         <v>19</v>
       </c>
       <c r="B123" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C123" t="s">
         <v>25</v>
@@ -2491,7 +2489,7 @@
         <v>19</v>
       </c>
       <c r="B124" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C124" t="s">
         <v>25</v>
@@ -2505,10 +2503,10 @@
         <v>19</v>
       </c>
       <c r="B125" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C125" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D125" t="s">
         <v>10</v>
@@ -2519,10 +2517,10 @@
         <v>19</v>
       </c>
       <c r="B126" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C126" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D126" t="s">
         <v>10</v>
@@ -2533,10 +2531,10 @@
         <v>19</v>
       </c>
       <c r="B127" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C127" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D127" t="s">
         <v>10</v>
@@ -2547,10 +2545,10 @@
         <v>19</v>
       </c>
       <c r="B128" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C128" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D128" t="s">
         <v>10</v>
@@ -2558,16 +2556,19 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B129" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C129" t="s">
-        <v>31</v>
-      </c>
-      <c r="D129" t="s">
-        <v>10</v>
+        <v>25</v>
+      </c>
+      <c r="D129">
+        <v>26.294005679335001</v>
+      </c>
+      <c r="E129">
+        <v>12</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -2575,16 +2576,16 @@
         <v>20</v>
       </c>
       <c r="B130" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C130" t="s">
         <v>25</v>
       </c>
       <c r="D130">
-        <v>26.294005679335001</v>
+        <v>31.330797003598601</v>
       </c>
       <c r="E130">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -2592,7 +2593,7 @@
         <v>20</v>
       </c>
       <c r="B131" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C131" t="s">
         <v>25</v>
@@ -2609,13 +2610,13 @@
         <v>20</v>
       </c>
       <c r="B132" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C132" t="s">
         <v>25</v>
       </c>
       <c r="D132">
-        <v>31.330797003598601</v>
+        <v>29.699304983972301</v>
       </c>
       <c r="E132">
         <v>3</v>
@@ -2626,16 +2627,16 @@
         <v>20</v>
       </c>
       <c r="B133" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C133" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D133">
-        <v>29.699304983972301</v>
+        <v>26.294005679335001</v>
       </c>
       <c r="E133">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -2643,16 +2644,16 @@
         <v>20</v>
       </c>
       <c r="B134" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C134" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D134">
-        <v>26.294005679335001</v>
+        <v>31.330797003598601</v>
       </c>
       <c r="E134">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -2660,10 +2661,10 @@
         <v>20</v>
       </c>
       <c r="B135" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C135" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D135">
         <v>31.330797003598601</v>
@@ -2677,13 +2678,13 @@
         <v>20</v>
       </c>
       <c r="B136" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C136" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D136">
-        <v>31.330797003598601</v>
+        <v>29.699304983972301</v>
       </c>
       <c r="E136">
         <v>3</v>
@@ -2691,16 +2692,16 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B137" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C137" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D137">
-        <v>29.699304983972301</v>
+        <v>12.093368739633799</v>
       </c>
       <c r="E137">
         <v>2</v>
@@ -2711,7 +2712,7 @@
         <v>2</v>
       </c>
       <c r="B138" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C138" t="s">
         <v>25</v>
@@ -2728,7 +2729,7 @@
         <v>2</v>
       </c>
       <c r="B139" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C139" t="s">
         <v>25</v>
@@ -2745,7 +2746,7 @@
         <v>2</v>
       </c>
       <c r="B140" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C140" t="s">
         <v>25</v>
@@ -2754,7 +2755,7 @@
         <v>12.093368739633799</v>
       </c>
       <c r="E140">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -2762,16 +2763,16 @@
         <v>2</v>
       </c>
       <c r="B141" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C141" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D141">
         <v>12.093368739633799</v>
       </c>
       <c r="E141">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -2779,10 +2780,10 @@
         <v>2</v>
       </c>
       <c r="B142" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C142" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D142">
         <v>12.093368739633799</v>
@@ -2796,10 +2797,10 @@
         <v>2</v>
       </c>
       <c r="B143" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C143" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D143">
         <v>12.093368739633799</v>
@@ -2813,33 +2814,33 @@
         <v>2</v>
       </c>
       <c r="B144" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C144" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D144">
         <v>12.093368739633799</v>
       </c>
       <c r="E144">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B145" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C145" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D145">
-        <v>12.093368739633799</v>
+        <v>29.949979386555899</v>
       </c>
       <c r="E145">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -2847,16 +2848,16 @@
         <v>7</v>
       </c>
       <c r="B146" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C146" t="s">
         <v>25</v>
       </c>
       <c r="D146">
-        <v>29.949979386555899</v>
+        <v>36.6118591069324</v>
       </c>
       <c r="E146">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -2864,7 +2865,7 @@
         <v>7</v>
       </c>
       <c r="B147" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C147" t="s">
         <v>25</v>
@@ -2881,13 +2882,13 @@
         <v>7</v>
       </c>
       <c r="B148" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C148" t="s">
         <v>25</v>
       </c>
       <c r="D148">
-        <v>36.6118591069324</v>
+        <v>29.949979386555899</v>
       </c>
       <c r="E148">
         <v>4</v>
@@ -2898,16 +2899,16 @@
         <v>7</v>
       </c>
       <c r="B149" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C149" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D149">
         <v>29.949979386555899</v>
       </c>
       <c r="E149">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -2915,16 +2916,16 @@
         <v>7</v>
       </c>
       <c r="B150" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C150" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D150">
         <v>29.949979386555899</v>
       </c>
       <c r="E150">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -2932,10 +2933,10 @@
         <v>7</v>
       </c>
       <c r="B151" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C151" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D151">
         <v>29.949979386555899</v>
@@ -2949,33 +2950,33 @@
         <v>7</v>
       </c>
       <c r="B152" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C152" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D152">
         <v>29.949979386555899</v>
       </c>
       <c r="E152">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B153" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C153" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D153">
-        <v>29.949979386555899</v>
+        <v>11.313708498984701</v>
       </c>
       <c r="E153">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -2983,7 +2984,7 @@
         <v>0</v>
       </c>
       <c r="B154" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C154" t="s">
         <v>25</v>
@@ -3000,7 +3001,7 @@
         <v>0</v>
       </c>
       <c r="B155" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C155" t="s">
         <v>25</v>
@@ -3017,7 +3018,7 @@
         <v>0</v>
       </c>
       <c r="B156" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C156" t="s">
         <v>25</v>
@@ -3026,7 +3027,7 @@
         <v>11.313708498984701</v>
       </c>
       <c r="E156">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -3034,16 +3035,16 @@
         <v>0</v>
       </c>
       <c r="B157" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C157" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D157">
         <v>11.313708498984701</v>
       </c>
       <c r="E157">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -3051,10 +3052,10 @@
         <v>0</v>
       </c>
       <c r="B158" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C158" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D158">
         <v>11.313708498984701</v>
@@ -3068,10 +3069,10 @@
         <v>0</v>
       </c>
       <c r="B159" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C159" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D159">
         <v>11.313708498984701</v>
@@ -3085,37 +3086,20 @@
         <v>0</v>
       </c>
       <c r="B160" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C160" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D160">
         <v>11.313708498984701</v>
       </c>
       <c r="E160">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>0</v>
-      </c>
-      <c r="B161" t="s">
-        <v>24</v>
-      </c>
-      <c r="C161" t="s">
-        <v>31</v>
-      </c>
-      <c r="D161">
-        <v>11.313708498984701</v>
-      </c>
-      <c r="E161">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:E161">
+  <sortState ref="A1:E160">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added page on excel file with all data
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -12,14 +12,16 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8820"/>
   </bookViews>
   <sheets>
-    <sheet name="ASt" sheetId="1" r:id="rId1"/>
-    <sheet name="GBF" sheetId="4" r:id="rId2"/>
-    <sheet name="Classic Hillclimbing" sheetId="3" r:id="rId3"/>
-    <sheet name="2-Lookahead Hill Climbing" sheetId="2" r:id="rId4"/>
+    <sheet name="All" sheetId="5" r:id="rId1"/>
+    <sheet name="ASt" sheetId="1" r:id="rId2"/>
+    <sheet name="GBF" sheetId="4" r:id="rId3"/>
+    <sheet name="Classic Hillclimbing" sheetId="3" r:id="rId4"/>
+    <sheet name="2-Lookahead Hill Climbing" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="output" localSheetId="0">ASt!$A$1:$D$81</definedName>
-    <definedName name="output_1" localSheetId="0">ASt!$A$1:$D$40</definedName>
+    <definedName name="output" localSheetId="0">All!$A$1:$E$160</definedName>
+    <definedName name="output" localSheetId="1">ASt!$A$1:$D$81</definedName>
+    <definedName name="output_1" localSheetId="1">ASt!$A$1:$D$40</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -54,11 +56,22 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="3" name="output2" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\Ananda\Documents\ai-final-project-path-navigation\output\output.txt" tab="0" comma="1" delimiter="(">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="27">
   <si>
     <t xml:space="preserve">Trivial Case </t>
   </si>
@@ -128,6 +141,18 @@
   <si>
     <t>lookahead</t>
   </si>
+  <si>
+    <t>ASt</t>
+  </si>
+  <si>
+    <t>GBF</t>
+  </si>
+  <si>
+    <t>Classic hillclimbing</t>
+  </si>
+  <si>
+    <t>2-lookahead hillclimbing</t>
+  </si>
 </sst>
 </file>
 
@@ -182,10 +207,14 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="output" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="output_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="output" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -486,10 +515,2624 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E160"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="B129" sqref="B129:E136"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3">
+        <v>12.3584854723722</v>
+      </c>
+      <c r="E3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4">
+        <v>12.3584854723722</v>
+      </c>
+      <c r="E4">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9">
+        <v>12.6491106406735</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>12.6491106406735</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11">
+        <v>12.6491106406735</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12">
+        <v>12.6491106406735</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13">
+        <v>12.6491106406735</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14">
+        <v>12.6491106406735</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15">
+        <v>12.6491106406735</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16">
+        <v>12.6491106406735</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19">
+        <v>30.488451223761</v>
+      </c>
+      <c r="E19">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20">
+        <v>30.488451223761</v>
+      </c>
+      <c r="E20">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25">
+        <v>1320.0199923026801</v>
+      </c>
+      <c r="E25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26">
+        <v>1320.0199923026801</v>
+      </c>
+      <c r="E26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27">
+        <v>1051.7556884513599</v>
+      </c>
+      <c r="E27">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28">
+        <v>1051.7556884513599</v>
+      </c>
+      <c r="E28">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29">
+        <v>1201.7698730432801</v>
+      </c>
+      <c r="E29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30">
+        <v>1201.7698730432801</v>
+      </c>
+      <c r="E30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31">
+        <v>1201.7698730432801</v>
+      </c>
+      <c r="E31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32">
+        <v>1201.7698730432801</v>
+      </c>
+      <c r="E32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33">
+        <v>42.365635077180997</v>
+      </c>
+      <c r="E33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34">
+        <v>39.705281007208796</v>
+      </c>
+      <c r="E34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35">
+        <v>32.387650199806799</v>
+      </c>
+      <c r="E35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36">
+        <v>32.387650199806799</v>
+      </c>
+      <c r="E36">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41">
+        <v>31.483123626630402</v>
+      </c>
+      <c r="E41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42">
+        <v>31.483123626630402</v>
+      </c>
+      <c r="E42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45">
+        <v>31.483123626630402</v>
+      </c>
+      <c r="E45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46">
+        <v>31.483123626630402</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47">
+        <v>31.483123626630402</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" t="s">
+        <v>22</v>
+      </c>
+      <c r="D48">
+        <v>31.483123626630402</v>
+      </c>
+      <c r="E48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49">
+        <v>33.6422423646966</v>
+      </c>
+      <c r="E49">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50" t="s">
+        <v>22</v>
+      </c>
+      <c r="D50">
+        <v>33.6422423646966</v>
+      </c>
+      <c r="E50">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" t="s">
+        <v>21</v>
+      </c>
+      <c r="D51">
+        <v>30.8600945056786</v>
+      </c>
+      <c r="E51">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" t="s">
+        <v>23</v>
+      </c>
+      <c r="C52" t="s">
+        <v>22</v>
+      </c>
+      <c r="D52">
+        <v>30.8600945056786</v>
+      </c>
+      <c r="E52">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53" t="s">
+        <v>25</v>
+      </c>
+      <c r="C53" t="s">
+        <v>21</v>
+      </c>
+      <c r="D53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" t="s">
+        <v>25</v>
+      </c>
+      <c r="C54" t="s">
+        <v>22</v>
+      </c>
+      <c r="D54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>10</v>
+      </c>
+      <c r="B55" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" t="s">
+        <v>21</v>
+      </c>
+      <c r="D55">
+        <v>35.3903064624919</v>
+      </c>
+      <c r="E55">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>10</v>
+      </c>
+      <c r="B56" t="s">
+        <v>24</v>
+      </c>
+      <c r="C56" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56">
+        <v>35.3903064624919</v>
+      </c>
+      <c r="E56">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>11</v>
+      </c>
+      <c r="B57" t="s">
+        <v>26</v>
+      </c>
+      <c r="C57" t="s">
+        <v>21</v>
+      </c>
+      <c r="D57">
+        <v>37.027756377319903</v>
+      </c>
+      <c r="E57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>11</v>
+      </c>
+      <c r="B58" t="s">
+        <v>26</v>
+      </c>
+      <c r="C58" t="s">
+        <v>22</v>
+      </c>
+      <c r="D58">
+        <v>37.027756377319903</v>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>11</v>
+      </c>
+      <c r="B59" t="s">
+        <v>23</v>
+      </c>
+      <c r="C59" t="s">
+        <v>21</v>
+      </c>
+      <c r="D59">
+        <v>28.5643537898574</v>
+      </c>
+      <c r="E59">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>11</v>
+      </c>
+      <c r="B60" t="s">
+        <v>23</v>
+      </c>
+      <c r="C60" t="s">
+        <v>22</v>
+      </c>
+      <c r="D60">
+        <v>28.5643537898574</v>
+      </c>
+      <c r="E60">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>11</v>
+      </c>
+      <c r="B61" t="s">
+        <v>25</v>
+      </c>
+      <c r="C61" t="s">
+        <v>21</v>
+      </c>
+      <c r="D61">
+        <v>37.027756377319903</v>
+      </c>
+      <c r="E61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>11</v>
+      </c>
+      <c r="B62" t="s">
+        <v>25</v>
+      </c>
+      <c r="C62" t="s">
+        <v>22</v>
+      </c>
+      <c r="D62">
+        <v>37.027756377319903</v>
+      </c>
+      <c r="E62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>11</v>
+      </c>
+      <c r="B63" t="s">
+        <v>24</v>
+      </c>
+      <c r="C63" t="s">
+        <v>21</v>
+      </c>
+      <c r="D63">
+        <v>37.027756377319903</v>
+      </c>
+      <c r="E63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>11</v>
+      </c>
+      <c r="B64" t="s">
+        <v>24</v>
+      </c>
+      <c r="C64" t="s">
+        <v>22</v>
+      </c>
+      <c r="D64">
+        <v>37.027756377319903</v>
+      </c>
+      <c r="E64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65" t="s">
+        <v>26</v>
+      </c>
+      <c r="C65" t="s">
+        <v>21</v>
+      </c>
+      <c r="D65">
+        <v>37.498733967920998</v>
+      </c>
+      <c r="E65">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>12</v>
+      </c>
+      <c r="B66" t="s">
+        <v>26</v>
+      </c>
+      <c r="C66" t="s">
+        <v>22</v>
+      </c>
+      <c r="D66">
+        <v>37.498733967920998</v>
+      </c>
+      <c r="E66">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>12</v>
+      </c>
+      <c r="B67" t="s">
+        <v>23</v>
+      </c>
+      <c r="C67" t="s">
+        <v>21</v>
+      </c>
+      <c r="D67">
+        <v>30.7861570503702</v>
+      </c>
+      <c r="E67">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>12</v>
+      </c>
+      <c r="B68" t="s">
+        <v>23</v>
+      </c>
+      <c r="C68" t="s">
+        <v>22</v>
+      </c>
+      <c r="D68">
+        <v>30.7861570503702</v>
+      </c>
+      <c r="E68">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>12</v>
+      </c>
+      <c r="B69" t="s">
+        <v>25</v>
+      </c>
+      <c r="C69" t="s">
+        <v>21</v>
+      </c>
+      <c r="D69">
+        <v>34.292985660078799</v>
+      </c>
+      <c r="E69">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>12</v>
+      </c>
+      <c r="B70" t="s">
+        <v>25</v>
+      </c>
+      <c r="C70" t="s">
+        <v>22</v>
+      </c>
+      <c r="D70">
+        <v>37.498733967920998</v>
+      </c>
+      <c r="E70">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>12</v>
+      </c>
+      <c r="B71" t="s">
+        <v>24</v>
+      </c>
+      <c r="C71" t="s">
+        <v>21</v>
+      </c>
+      <c r="D71">
+        <v>37.498733967920998</v>
+      </c>
+      <c r="E71">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>12</v>
+      </c>
+      <c r="B72" t="s">
+        <v>24</v>
+      </c>
+      <c r="C72" t="s">
+        <v>22</v>
+      </c>
+      <c r="D72">
+        <v>34.292985660078799</v>
+      </c>
+      <c r="E72">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>13</v>
+      </c>
+      <c r="B73" t="s">
+        <v>26</v>
+      </c>
+      <c r="C73" t="s">
+        <v>21</v>
+      </c>
+      <c r="D73">
+        <v>29.9822657255168</v>
+      </c>
+      <c r="E73">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>13</v>
+      </c>
+      <c r="B74" t="s">
+        <v>26</v>
+      </c>
+      <c r="C74" t="s">
+        <v>22</v>
+      </c>
+      <c r="D74">
+        <v>32.252697129720197</v>
+      </c>
+      <c r="E74">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>13</v>
+      </c>
+      <c r="B75" t="s">
+        <v>23</v>
+      </c>
+      <c r="C75" t="s">
+        <v>21</v>
+      </c>
+      <c r="D75">
+        <v>29.2069904766599</v>
+      </c>
+      <c r="E75">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>13</v>
+      </c>
+      <c r="B76" t="s">
+        <v>23</v>
+      </c>
+      <c r="C76" t="s">
+        <v>22</v>
+      </c>
+      <c r="D76">
+        <v>29.2069904766599</v>
+      </c>
+      <c r="E76">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>13</v>
+      </c>
+      <c r="B77" t="s">
+        <v>25</v>
+      </c>
+      <c r="C77" t="s">
+        <v>21</v>
+      </c>
+      <c r="D77" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>13</v>
+      </c>
+      <c r="B78" t="s">
+        <v>25</v>
+      </c>
+      <c r="C78" t="s">
+        <v>22</v>
+      </c>
+      <c r="D78" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>13</v>
+      </c>
+      <c r="B79" t="s">
+        <v>24</v>
+      </c>
+      <c r="C79" t="s">
+        <v>21</v>
+      </c>
+      <c r="D79">
+        <v>30.804112043605901</v>
+      </c>
+      <c r="E79">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>13</v>
+      </c>
+      <c r="B80" t="s">
+        <v>24</v>
+      </c>
+      <c r="C80" t="s">
+        <v>22</v>
+      </c>
+      <c r="D80">
+        <v>30.804112043605901</v>
+      </c>
+      <c r="E80">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>3</v>
+      </c>
+      <c r="B81" t="s">
+        <v>26</v>
+      </c>
+      <c r="C81" t="s">
+        <v>21</v>
+      </c>
+      <c r="D81">
+        <v>12.6491106406735</v>
+      </c>
+      <c r="E81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>3</v>
+      </c>
+      <c r="B82" t="s">
+        <v>26</v>
+      </c>
+      <c r="C82" t="s">
+        <v>22</v>
+      </c>
+      <c r="D82">
+        <v>12.6491106406735</v>
+      </c>
+      <c r="E82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>3</v>
+      </c>
+      <c r="B83" t="s">
+        <v>23</v>
+      </c>
+      <c r="C83" t="s">
+        <v>21</v>
+      </c>
+      <c r="D83">
+        <v>11.313708498984701</v>
+      </c>
+      <c r="E83">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>3</v>
+      </c>
+      <c r="B84" t="s">
+        <v>23</v>
+      </c>
+      <c r="C84" t="s">
+        <v>22</v>
+      </c>
+      <c r="D84">
+        <v>11.313708498984701</v>
+      </c>
+      <c r="E84">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>3</v>
+      </c>
+      <c r="B85" t="s">
+        <v>25</v>
+      </c>
+      <c r="C85" t="s">
+        <v>21</v>
+      </c>
+      <c r="D85">
+        <v>12.6491106406735</v>
+      </c>
+      <c r="E85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>3</v>
+      </c>
+      <c r="B86" t="s">
+        <v>25</v>
+      </c>
+      <c r="C86" t="s">
+        <v>22</v>
+      </c>
+      <c r="D86">
+        <v>12.6491106406735</v>
+      </c>
+      <c r="E86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>3</v>
+      </c>
+      <c r="B87" t="s">
+        <v>24</v>
+      </c>
+      <c r="C87" t="s">
+        <v>21</v>
+      </c>
+      <c r="D87">
+        <v>12.6491106406735</v>
+      </c>
+      <c r="E87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>3</v>
+      </c>
+      <c r="B88" t="s">
+        <v>24</v>
+      </c>
+      <c r="C88" t="s">
+        <v>22</v>
+      </c>
+      <c r="D88">
+        <v>12.6491106406735</v>
+      </c>
+      <c r="E88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>14</v>
+      </c>
+      <c r="B89" t="s">
+        <v>26</v>
+      </c>
+      <c r="C89" t="s">
+        <v>21</v>
+      </c>
+      <c r="D89">
+        <v>35.038404810405297</v>
+      </c>
+      <c r="E89">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>14</v>
+      </c>
+      <c r="B90" t="s">
+        <v>26</v>
+      </c>
+      <c r="C90" t="s">
+        <v>22</v>
+      </c>
+      <c r="D90">
+        <v>35.038404810405297</v>
+      </c>
+      <c r="E90">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>14</v>
+      </c>
+      <c r="B91" t="s">
+        <v>23</v>
+      </c>
+      <c r="C91" t="s">
+        <v>21</v>
+      </c>
+      <c r="D91">
+        <v>29.2409415537572</v>
+      </c>
+      <c r="E91">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>14</v>
+      </c>
+      <c r="B92" t="s">
+        <v>23</v>
+      </c>
+      <c r="C92" t="s">
+        <v>22</v>
+      </c>
+      <c r="D92">
+        <v>29.2409415537572</v>
+      </c>
+      <c r="E92">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>14</v>
+      </c>
+      <c r="B93" t="s">
+        <v>25</v>
+      </c>
+      <c r="C93" t="s">
+        <v>21</v>
+      </c>
+      <c r="D93">
+        <v>32.320626387486001</v>
+      </c>
+      <c r="E93">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>14</v>
+      </c>
+      <c r="B94" t="s">
+        <v>25</v>
+      </c>
+      <c r="C94" t="s">
+        <v>22</v>
+      </c>
+      <c r="D94">
+        <v>32.320626387486001</v>
+      </c>
+      <c r="E94">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>14</v>
+      </c>
+      <c r="B95" t="s">
+        <v>24</v>
+      </c>
+      <c r="C95" t="s">
+        <v>21</v>
+      </c>
+      <c r="D95">
+        <v>32.320626387486001</v>
+      </c>
+      <c r="E95">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>14</v>
+      </c>
+      <c r="B96" t="s">
+        <v>24</v>
+      </c>
+      <c r="C96" t="s">
+        <v>22</v>
+      </c>
+      <c r="D96">
+        <v>32.320626387486001</v>
+      </c>
+      <c r="E96">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>15</v>
+      </c>
+      <c r="B97" t="s">
+        <v>26</v>
+      </c>
+      <c r="C97" t="s">
+        <v>21</v>
+      </c>
+      <c r="D97" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>15</v>
+      </c>
+      <c r="B98" t="s">
+        <v>26</v>
+      </c>
+      <c r="C98" t="s">
+        <v>22</v>
+      </c>
+      <c r="D98" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>15</v>
+      </c>
+      <c r="B99" t="s">
+        <v>23</v>
+      </c>
+      <c r="C99" t="s">
+        <v>21</v>
+      </c>
+      <c r="D99">
+        <v>30.427603346441899</v>
+      </c>
+      <c r="E99">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>15</v>
+      </c>
+      <c r="B100" t="s">
+        <v>23</v>
+      </c>
+      <c r="C100" t="s">
+        <v>22</v>
+      </c>
+      <c r="D100">
+        <v>30.427603346441899</v>
+      </c>
+      <c r="E100">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>15</v>
+      </c>
+      <c r="B101" t="s">
+        <v>25</v>
+      </c>
+      <c r="C101" t="s">
+        <v>21</v>
+      </c>
+      <c r="D101" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>15</v>
+      </c>
+      <c r="B102" t="s">
+        <v>25</v>
+      </c>
+      <c r="C102" t="s">
+        <v>22</v>
+      </c>
+      <c r="D102" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>15</v>
+      </c>
+      <c r="B103" t="s">
+        <v>24</v>
+      </c>
+      <c r="C103" t="s">
+        <v>21</v>
+      </c>
+      <c r="D103" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>15</v>
+      </c>
+      <c r="B104" t="s">
+        <v>24</v>
+      </c>
+      <c r="C104" t="s">
+        <v>22</v>
+      </c>
+      <c r="D104" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>16</v>
+      </c>
+      <c r="B105" t="s">
+        <v>26</v>
+      </c>
+      <c r="C105" t="s">
+        <v>21</v>
+      </c>
+      <c r="D105" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>16</v>
+      </c>
+      <c r="B106" t="s">
+        <v>26</v>
+      </c>
+      <c r="C106" t="s">
+        <v>22</v>
+      </c>
+      <c r="D106" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>16</v>
+      </c>
+      <c r="B107" t="s">
+        <v>23</v>
+      </c>
+      <c r="C107" t="s">
+        <v>21</v>
+      </c>
+      <c r="D107" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>16</v>
+      </c>
+      <c r="B108" t="s">
+        <v>23</v>
+      </c>
+      <c r="C108" t="s">
+        <v>22</v>
+      </c>
+      <c r="D108" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>16</v>
+      </c>
+      <c r="B109" t="s">
+        <v>25</v>
+      </c>
+      <c r="C109" t="s">
+        <v>21</v>
+      </c>
+      <c r="D109" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>16</v>
+      </c>
+      <c r="B110" t="s">
+        <v>25</v>
+      </c>
+      <c r="C110" t="s">
+        <v>22</v>
+      </c>
+      <c r="D110" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>16</v>
+      </c>
+      <c r="B111" t="s">
+        <v>24</v>
+      </c>
+      <c r="C111" t="s">
+        <v>21</v>
+      </c>
+      <c r="D111" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>16</v>
+      </c>
+      <c r="B112" t="s">
+        <v>24</v>
+      </c>
+      <c r="C112" t="s">
+        <v>22</v>
+      </c>
+      <c r="D112" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>17</v>
+      </c>
+      <c r="B113" t="s">
+        <v>26</v>
+      </c>
+      <c r="C113" t="s">
+        <v>21</v>
+      </c>
+      <c r="D113">
+        <v>31.521347176340399</v>
+      </c>
+      <c r="E113">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>17</v>
+      </c>
+      <c r="B114" t="s">
+        <v>26</v>
+      </c>
+      <c r="C114" t="s">
+        <v>22</v>
+      </c>
+      <c r="D114">
+        <v>31.521347176340399</v>
+      </c>
+      <c r="E114">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>17</v>
+      </c>
+      <c r="B115" t="s">
+        <v>23</v>
+      </c>
+      <c r="C115" t="s">
+        <v>21</v>
+      </c>
+      <c r="D115">
+        <v>31.521347176340399</v>
+      </c>
+      <c r="E115">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>17</v>
+      </c>
+      <c r="B116" t="s">
+        <v>23</v>
+      </c>
+      <c r="C116" t="s">
+        <v>22</v>
+      </c>
+      <c r="D116">
+        <v>31.521347176340399</v>
+      </c>
+      <c r="E116">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>17</v>
+      </c>
+      <c r="B117" t="s">
+        <v>25</v>
+      </c>
+      <c r="C117" t="s">
+        <v>21</v>
+      </c>
+      <c r="D117">
+        <v>32.748605090273202</v>
+      </c>
+      <c r="E117">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>17</v>
+      </c>
+      <c r="B118" t="s">
+        <v>25</v>
+      </c>
+      <c r="C118" t="s">
+        <v>22</v>
+      </c>
+      <c r="D118">
+        <v>32.748605090273202</v>
+      </c>
+      <c r="E118">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>17</v>
+      </c>
+      <c r="B119" t="s">
+        <v>24</v>
+      </c>
+      <c r="C119" t="s">
+        <v>21</v>
+      </c>
+      <c r="D119">
+        <v>32.748605090273202</v>
+      </c>
+      <c r="E119">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>17</v>
+      </c>
+      <c r="B120" t="s">
+        <v>24</v>
+      </c>
+      <c r="C120" t="s">
+        <v>22</v>
+      </c>
+      <c r="D120">
+        <v>32.748605090273202</v>
+      </c>
+      <c r="E120">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>18</v>
+      </c>
+      <c r="B121" t="s">
+        <v>26</v>
+      </c>
+      <c r="C121" t="s">
+        <v>21</v>
+      </c>
+      <c r="D121" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>18</v>
+      </c>
+      <c r="B122" t="s">
+        <v>26</v>
+      </c>
+      <c r="C122" t="s">
+        <v>22</v>
+      </c>
+      <c r="D122" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>18</v>
+      </c>
+      <c r="B123" t="s">
+        <v>23</v>
+      </c>
+      <c r="C123" t="s">
+        <v>21</v>
+      </c>
+      <c r="D123" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>18</v>
+      </c>
+      <c r="B124" t="s">
+        <v>23</v>
+      </c>
+      <c r="C124" t="s">
+        <v>22</v>
+      </c>
+      <c r="D124" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>18</v>
+      </c>
+      <c r="B125" t="s">
+        <v>25</v>
+      </c>
+      <c r="C125" t="s">
+        <v>21</v>
+      </c>
+      <c r="D125" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>18</v>
+      </c>
+      <c r="B126" t="s">
+        <v>25</v>
+      </c>
+      <c r="C126" t="s">
+        <v>22</v>
+      </c>
+      <c r="D126" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>18</v>
+      </c>
+      <c r="B127" t="s">
+        <v>24</v>
+      </c>
+      <c r="C127" t="s">
+        <v>21</v>
+      </c>
+      <c r="D127" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>18</v>
+      </c>
+      <c r="B128" t="s">
+        <v>24</v>
+      </c>
+      <c r="C128" t="s">
+        <v>22</v>
+      </c>
+      <c r="D128" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>19</v>
+      </c>
+      <c r="B129" t="s">
+        <v>26</v>
+      </c>
+      <c r="C129" t="s">
+        <v>21</v>
+      </c>
+      <c r="D129">
+        <v>29.699304983972301</v>
+      </c>
+      <c r="E129">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>19</v>
+      </c>
+      <c r="B130" t="s">
+        <v>26</v>
+      </c>
+      <c r="C130" t="s">
+        <v>22</v>
+      </c>
+      <c r="D130">
+        <v>29.699304983972301</v>
+      </c>
+      <c r="E130">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>19</v>
+      </c>
+      <c r="B131" t="s">
+        <v>23</v>
+      </c>
+      <c r="C131" t="s">
+        <v>21</v>
+      </c>
+      <c r="D131">
+        <v>26.294005679335001</v>
+      </c>
+      <c r="E131">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>19</v>
+      </c>
+      <c r="B132" t="s">
+        <v>23</v>
+      </c>
+      <c r="C132" t="s">
+        <v>22</v>
+      </c>
+      <c r="D132">
+        <v>26.294005679335001</v>
+      </c>
+      <c r="E132">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>19</v>
+      </c>
+      <c r="B133" t="s">
+        <v>25</v>
+      </c>
+      <c r="C133" t="s">
+        <v>21</v>
+      </c>
+      <c r="D133">
+        <v>31.330797003598601</v>
+      </c>
+      <c r="E133">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>19</v>
+      </c>
+      <c r="B134" t="s">
+        <v>25</v>
+      </c>
+      <c r="C134" t="s">
+        <v>22</v>
+      </c>
+      <c r="D134">
+        <v>31.330797003598601</v>
+      </c>
+      <c r="E134">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>19</v>
+      </c>
+      <c r="B135" t="s">
+        <v>24</v>
+      </c>
+      <c r="C135" t="s">
+        <v>21</v>
+      </c>
+      <c r="D135">
+        <v>31.330797003598601</v>
+      </c>
+      <c r="E135">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>19</v>
+      </c>
+      <c r="B136" t="s">
+        <v>24</v>
+      </c>
+      <c r="C136" t="s">
+        <v>22</v>
+      </c>
+      <c r="D136">
+        <v>31.330797003598601</v>
+      </c>
+      <c r="E136">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>1</v>
+      </c>
+      <c r="B137" t="s">
+        <v>26</v>
+      </c>
+      <c r="C137" t="s">
+        <v>21</v>
+      </c>
+      <c r="D137">
+        <v>12.093368739633799</v>
+      </c>
+      <c r="E137">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>1</v>
+      </c>
+      <c r="B138" t="s">
+        <v>26</v>
+      </c>
+      <c r="C138" t="s">
+        <v>22</v>
+      </c>
+      <c r="D138">
+        <v>12.093368739633799</v>
+      </c>
+      <c r="E138">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>1</v>
+      </c>
+      <c r="B139" t="s">
+        <v>23</v>
+      </c>
+      <c r="C139" t="s">
+        <v>21</v>
+      </c>
+      <c r="D139">
+        <v>12.093368739633799</v>
+      </c>
+      <c r="E139">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>1</v>
+      </c>
+      <c r="B140" t="s">
+        <v>23</v>
+      </c>
+      <c r="C140" t="s">
+        <v>22</v>
+      </c>
+      <c r="D140">
+        <v>12.093368739633799</v>
+      </c>
+      <c r="E140">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>1</v>
+      </c>
+      <c r="B141" t="s">
+        <v>25</v>
+      </c>
+      <c r="C141" t="s">
+        <v>21</v>
+      </c>
+      <c r="D141">
+        <v>12.093368739633799</v>
+      </c>
+      <c r="E141">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>1</v>
+      </c>
+      <c r="B142" t="s">
+        <v>25</v>
+      </c>
+      <c r="C142" t="s">
+        <v>22</v>
+      </c>
+      <c r="D142">
+        <v>12.093368739633799</v>
+      </c>
+      <c r="E142">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>1</v>
+      </c>
+      <c r="B143" t="s">
+        <v>24</v>
+      </c>
+      <c r="C143" t="s">
+        <v>21</v>
+      </c>
+      <c r="D143">
+        <v>12.093368739633799</v>
+      </c>
+      <c r="E143">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>1</v>
+      </c>
+      <c r="B144" t="s">
+        <v>24</v>
+      </c>
+      <c r="C144" t="s">
+        <v>22</v>
+      </c>
+      <c r="D144">
+        <v>12.093368739633799</v>
+      </c>
+      <c r="E144">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>6</v>
+      </c>
+      <c r="B145" t="s">
+        <v>26</v>
+      </c>
+      <c r="C145" t="s">
+        <v>21</v>
+      </c>
+      <c r="D145">
+        <v>29.949979386555899</v>
+      </c>
+      <c r="E145">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>6</v>
+      </c>
+      <c r="B146" t="s">
+        <v>26</v>
+      </c>
+      <c r="C146" t="s">
+        <v>22</v>
+      </c>
+      <c r="D146">
+        <v>29.949979386555899</v>
+      </c>
+      <c r="E146">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>6</v>
+      </c>
+      <c r="B147" t="s">
+        <v>23</v>
+      </c>
+      <c r="C147" t="s">
+        <v>21</v>
+      </c>
+      <c r="D147">
+        <v>29.949979386555899</v>
+      </c>
+      <c r="E147">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>6</v>
+      </c>
+      <c r="B148" t="s">
+        <v>23</v>
+      </c>
+      <c r="C148" t="s">
+        <v>22</v>
+      </c>
+      <c r="D148">
+        <v>29.949979386555899</v>
+      </c>
+      <c r="E148">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>6</v>
+      </c>
+      <c r="B149" t="s">
+        <v>25</v>
+      </c>
+      <c r="C149" t="s">
+        <v>21</v>
+      </c>
+      <c r="D149">
+        <v>36.6118591069324</v>
+      </c>
+      <c r="E149">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>6</v>
+      </c>
+      <c r="B150" t="s">
+        <v>25</v>
+      </c>
+      <c r="C150" t="s">
+        <v>22</v>
+      </c>
+      <c r="D150">
+        <v>29.949979386555899</v>
+      </c>
+      <c r="E150">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>6</v>
+      </c>
+      <c r="B151" t="s">
+        <v>24</v>
+      </c>
+      <c r="C151" t="s">
+        <v>21</v>
+      </c>
+      <c r="D151">
+        <v>36.6118591069324</v>
+      </c>
+      <c r="E151">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>6</v>
+      </c>
+      <c r="B152" t="s">
+        <v>24</v>
+      </c>
+      <c r="C152" t="s">
+        <v>22</v>
+      </c>
+      <c r="D152">
+        <v>29.949979386555899</v>
+      </c>
+      <c r="E152">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>0</v>
+      </c>
+      <c r="B153" t="s">
+        <v>26</v>
+      </c>
+      <c r="C153" t="s">
+        <v>21</v>
+      </c>
+      <c r="D153">
+        <v>11.313708498984701</v>
+      </c>
+      <c r="E153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>0</v>
+      </c>
+      <c r="B154" t="s">
+        <v>26</v>
+      </c>
+      <c r="C154" t="s">
+        <v>22</v>
+      </c>
+      <c r="D154">
+        <v>11.313708498984701</v>
+      </c>
+      <c r="E154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>0</v>
+      </c>
+      <c r="B155" t="s">
+        <v>23</v>
+      </c>
+      <c r="C155" t="s">
+        <v>21</v>
+      </c>
+      <c r="D155">
+        <v>11.313708498984701</v>
+      </c>
+      <c r="E155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>0</v>
+      </c>
+      <c r="B156" t="s">
+        <v>23</v>
+      </c>
+      <c r="C156" t="s">
+        <v>22</v>
+      </c>
+      <c r="D156">
+        <v>11.313708498984701</v>
+      </c>
+      <c r="E156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>0</v>
+      </c>
+      <c r="B157" t="s">
+        <v>25</v>
+      </c>
+      <c r="C157" t="s">
+        <v>21</v>
+      </c>
+      <c r="D157">
+        <v>11.313708498984701</v>
+      </c>
+      <c r="E157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>0</v>
+      </c>
+      <c r="B158" t="s">
+        <v>25</v>
+      </c>
+      <c r="C158" t="s">
+        <v>22</v>
+      </c>
+      <c r="D158">
+        <v>11.313708498984701</v>
+      </c>
+      <c r="E158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>0</v>
+      </c>
+      <c r="B159" t="s">
+        <v>24</v>
+      </c>
+      <c r="C159" t="s">
+        <v>21</v>
+      </c>
+      <c r="D159">
+        <v>11.313708498984701</v>
+      </c>
+      <c r="E159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>0</v>
+      </c>
+      <c r="B160" t="s">
+        <v>24</v>
+      </c>
+      <c r="C160" t="s">
+        <v>22</v>
+      </c>
+      <c r="D160">
+        <v>11.313708498984701</v>
+      </c>
+      <c r="E160">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:E160">
+    <sortCondition ref="A3"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,545 +3691,6 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D40"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3">
-        <v>12.6491106406735</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4">
-        <v>12.6491106406735</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7">
-        <v>1201.7698730432801</v>
-      </c>
-      <c r="D7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8">
-        <v>1201.7698730432801</v>
-      </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11">
-        <v>31.483123626630402</v>
-      </c>
-      <c r="D11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12">
-        <v>31.483123626630402</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13">
-        <v>35.3903064624919</v>
-      </c>
-      <c r="D13">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14">
-        <v>35.3903064624919</v>
-      </c>
-      <c r="D14">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15">
-        <v>37.027756377319903</v>
-      </c>
-      <c r="D15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16">
-        <v>37.027756377319903</v>
-      </c>
-      <c r="D16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17">
-        <v>37.498733967920998</v>
-      </c>
-      <c r="D17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18">
-        <v>34.292985660078799</v>
-      </c>
-      <c r="D18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19">
-        <v>30.804112043605901</v>
-      </c>
-      <c r="D19">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20">
-        <v>30.804112043605901</v>
-      </c>
-      <c r="D20">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21">
-        <v>12.6491106406735</v>
-      </c>
-      <c r="D21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22">
-        <v>12.6491106406735</v>
-      </c>
-      <c r="D22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23">
-        <v>32.320626387486001</v>
-      </c>
-      <c r="D23">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24">
-        <v>32.320626387486001</v>
-      </c>
-      <c r="D24">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29">
-        <v>32.748605090273202</v>
-      </c>
-      <c r="D29">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" t="s">
-        <v>22</v>
-      </c>
-      <c r="C30">
-        <v>32.748605090273202</v>
-      </c>
-      <c r="D30">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B32" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>19</v>
-      </c>
-      <c r="B33" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33">
-        <v>31.330797003598601</v>
-      </c>
-      <c r="D33">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>19</v>
-      </c>
-      <c r="B34" t="s">
-        <v>22</v>
-      </c>
-      <c r="C34">
-        <v>31.330797003598601</v>
-      </c>
-      <c r="D34">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35">
-        <v>12.093368739633799</v>
-      </c>
-      <c r="D35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>1</v>
-      </c>
-      <c r="B36" t="s">
-        <v>22</v>
-      </c>
-      <c r="C36">
-        <v>12.093368739633799</v>
-      </c>
-      <c r="D36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" t="s">
-        <v>21</v>
-      </c>
-      <c r="C37">
-        <v>36.6118591069324</v>
-      </c>
-      <c r="D37">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" t="s">
-        <v>22</v>
-      </c>
-      <c r="C38">
-        <v>29.949979386555899</v>
-      </c>
-      <c r="D38">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>0</v>
-      </c>
-      <c r="B39" t="s">
-        <v>21</v>
-      </c>
-      <c r="C39">
-        <v>11.313708498984701</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" t="s">
-        <v>22</v>
-      </c>
-      <c r="C40">
-        <v>11.313708498984701</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1757,8 +3861,11 @@
       <c r="B13" t="s">
         <v>21</v>
       </c>
-      <c r="C13" t="s">
-        <v>9</v>
+      <c r="C13">
+        <v>35.3903064624919</v>
+      </c>
+      <c r="D13">
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1768,8 +3875,11 @@
       <c r="B14" t="s">
         <v>22</v>
       </c>
-      <c r="C14" t="s">
-        <v>9</v>
+      <c r="C14">
+        <v>35.3903064624919</v>
+      </c>
+      <c r="D14">
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1808,10 +3918,10 @@
         <v>21</v>
       </c>
       <c r="C17">
-        <v>34.292985660078799</v>
+        <v>37.498733967920998</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1822,10 +3932,10 @@
         <v>22</v>
       </c>
       <c r="C18">
-        <v>37.498733967920998</v>
+        <v>34.292985660078799</v>
       </c>
       <c r="D18">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1835,8 +3945,11 @@
       <c r="B19" t="s">
         <v>21</v>
       </c>
-      <c r="C19" t="s">
-        <v>9</v>
+      <c r="C19">
+        <v>30.804112043605901</v>
+      </c>
+      <c r="D19">
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1846,8 +3959,11 @@
       <c r="B20" t="s">
         <v>22</v>
       </c>
-      <c r="C20" t="s">
-        <v>9</v>
+      <c r="C20">
+        <v>30.804112043605901</v>
+      </c>
+      <c r="D20">
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2207,6 +4323,533 @@
         <v>21</v>
       </c>
       <c r="C7">
+        <v>1201.7698730432801</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8">
+        <v>1201.7698730432801</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>31.483123626630402</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12">
+        <v>31.483123626630402</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15">
+        <v>37.027756377319903</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16">
+        <v>37.027756377319903</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>34.292985660078799</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18">
+        <v>37.498733967920998</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21">
+        <v>12.6491106406735</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22">
+        <v>12.6491106406735</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23">
+        <v>32.320626387486001</v>
+      </c>
+      <c r="D23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>32.320626387486001</v>
+      </c>
+      <c r="D24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29">
+        <v>32.748605090273202</v>
+      </c>
+      <c r="D29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30">
+        <v>32.748605090273202</v>
+      </c>
+      <c r="D30">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33">
+        <v>31.330797003598601</v>
+      </c>
+      <c r="D33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34">
+        <v>31.330797003598601</v>
+      </c>
+      <c r="D34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35">
+        <v>12.093368739633799</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36">
+        <v>12.093368739633799</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37">
+        <v>36.6118591069324</v>
+      </c>
+      <c r="D37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38">
+        <v>29.949979386555899</v>
+      </c>
+      <c r="D38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39">
+        <v>11.313708498984701</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40">
+        <v>11.313708498984701</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>12.6491106406735</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4">
+        <v>12.6491106406735</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7">
         <v>1320.0199923026801</v>
       </c>
       <c r="D7">

</xml_diff>